<commit_message>
update data test for bmi, add class for page object
</commit_message>
<xml_diff>
--- a/datatest/dataForBMI.xlsx
+++ b/datatest/dataForBMI.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Age</t>
   </si>
@@ -44,20 +44,131 @@
     <t>Male</t>
   </si>
   <si>
-    <t>nothing</t>
+    <t>BMI = 13.9 kg/m2   (Severe thinness)</t>
+  </si>
+  <si>
+    <r>
+      <t>BMI = 15.9 kg/m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>   (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFB90606"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Severe thinness</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>BMI = 16 kg/m2   (Moderate thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 17 kg/m2   (Moderate thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 17.1 kg/m2   (Mild thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 18.5 kg/m2   (Mild thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 18.6 kg/m2   (Normal)</t>
+  </si>
+  <si>
+    <t>BMI = 25 kg/m2   (Normal)</t>
+  </si>
+  <si>
+    <t>BMI = 25.1 kg/m2   (Overweight)</t>
+  </si>
+  <si>
+    <t>BMI = 30 kg/m2   (Overweight)</t>
+  </si>
+  <si>
+    <t>BMI = 30.1 kg/m2   (Obese Class I)</t>
+  </si>
+  <si>
+    <t>BMI = 35 kg/m2   (Obese Class I)</t>
+  </si>
+  <si>
+    <t>BMI = 35.1 kg/m2   (Mild thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 40 kg/m2   (Mild thinness)</t>
+  </si>
+  <si>
+    <t>BMI = 40.1 kg/m2   (Mild thinness)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFB90606"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,8 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,15 +474,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="5" max="5" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -407,7 +519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>120</v>
       </c>
@@ -415,13 +527,13 @@
         <v>5</v>
       </c>
       <c r="C3">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D3">
-        <v>20</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+        <v>51.515999999999998</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -432,16 +544,221 @@
         <v>5</v>
       </c>
       <c r="C4">
+        <v>175</v>
+      </c>
+      <c r="D4">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>170</v>
+      </c>
+      <c r="D5">
+        <v>49.13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>190</v>
+      </c>
+      <c r="D6">
+        <v>61.731000000000002</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>190</v>
+      </c>
+      <c r="D7">
+        <v>66.784999999999997</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>190</v>
+      </c>
+      <c r="D8">
+        <v>67.146000000000001</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>190</v>
+      </c>
+      <c r="D9">
+        <v>90.25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>190</v>
+      </c>
+      <c r="D10">
+        <v>90.611000000000004</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>40</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
         <v>120</v>
       </c>
-      <c r="D4">
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>120.4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>200</v>
+      </c>
+      <c r="D13">
+        <v>140</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>200</v>
+      </c>
+      <c r="D14">
+        <v>140.4</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>200</v>
+      </c>
+      <c r="D15">
+        <v>160</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>200</v>
+      </c>
+      <c r="D16">
+        <v>160.4</v>
+      </c>
+      <c r="E16" t="s">
         <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>